<commit_message>
CCKH Update KH-Canteen-Edu/Fact._Gold and similar stores in template
</commit_message>
<xml_diff>
--- a/Projects/CCKH/Data/Template_New.xlsx
+++ b/Projects/CCKH/Data/Template_New.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,12 +32,16 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs!$A$1:$T$32</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIs!$A$1:$T$32</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIs!$A$1:$T$32</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$T$32</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$T$32</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">AVAILABILITY!$B$5:$CH$19</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$18</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$19</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$18</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$19</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$18</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">VISIBILITY!$B$5:$F$5</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">COOLER!$B$5:$S$5</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">COOLER!$B$5:$S$5</definedName>
@@ -45,6 +49,8 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">COOLER!$B$5:$S$5</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">COOLER!$B$5:$S$5</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">COOLER!$B$5:$S$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">COOLER!$B$5:$S$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">COOLER!$B$5:$S$5</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -56,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="231">
   <si>
     <t xml:space="preserve">Store Type</t>
   </si>
@@ -657,7 +663,7 @@
     <t xml:space="preserve">KH-BBQ/Soup/Beer Gdn_Gold</t>
   </si>
   <si>
-    <t xml:space="preserve">KH-Canteen-Edu/Fact_Gold</t>
+    <t xml:space="preserve">KH-Canteen-Edu/Fact._Gold</t>
   </si>
   <si>
     <t xml:space="preserve">KH-Food Stalls_Gold</t>
@@ -819,7 +825,7 @@
     <t xml:space="preserve">KH-BBQ/Soup/Beer Gdn_Bronze</t>
   </si>
   <si>
-    <t xml:space="preserve">KH-Canteen-Edu/Fact_Bronze</t>
+    <t xml:space="preserve">KH-Canteen-Edu/Fact._Bronze</t>
   </si>
   <si>
     <t xml:space="preserve">KH-Food Stalls_Bronze</t>
@@ -950,9 +956,6 @@
   </si>
   <si>
     <t xml:space="preserve">Weight Per Store Types (N/A - do not run KPI)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Canteen-Edu/Fact._Gold</t>
   </si>
 </sst>
 </file>
@@ -1673,29 +1676,29 @@
   </sheetPr>
   <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="G1" colorId="64" zoomScale="90" zoomScaleNormal="86" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O23" activeCellId="0" sqref="O23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="86" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.9919028340081"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.8137651821862"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.3846153846154"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="77.6599190283401"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="53.2388663967611"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.3481781376518"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.8137651821862"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="79.0526315789474"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="54.0931174089069"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="41.8825910931174"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="42.5263157894737"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="37.4898785425101"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="75.6275303643725"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="77.0202429149798"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="29.9919028340081"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="9.10526315789474"/>
@@ -3182,19 +3185,19 @@
   </sheetPr>
   <dimension ref="A1:CH19"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="AE1" colorId="64" zoomScale="90" zoomScaleNormal="70" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="V1" colorId="64" zoomScale="90" zoomScaleNormal="70" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="BE5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="AE1" activeCellId="0" sqref="AE1"/>
-      <selection pane="bottomLeft" activeCell="AI26" activeCellId="0" sqref="AI26"/>
+      <selection pane="topLeft" activeCell="V1" activeCellId="0" sqref="V1"/>
+      <selection pane="bottomLeft" activeCell="Z5" activeCellId="0" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="65.7692307692308"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.5627530364373"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="86" min="5" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="66.9473684210526"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.2024291497976"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="86" min="5" style="0" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="87" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -7330,14 +7333,14 @@
   </sheetPr>
   <dimension ref="B1:CF8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="85" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="AS1" colorId="64" zoomScale="90" zoomScaleNormal="85" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AY5" activeCellId="0" sqref="AY5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="57.8461538461538"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="58.8097165991903"/>
     <col collapsed="false" hidden="false" max="84" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="85" style="0" width="8.57085020242915"/>
   </cols>
@@ -7567,7 +7570,7 @@
         <v>132</v>
       </c>
       <c r="M5" s="30" t="s">
-        <v>231</v>
+        <v>133</v>
       </c>
       <c r="N5" s="30" t="s">
         <v>134</v>
@@ -8564,16 +8567,16 @@
   </sheetPr>
   <dimension ref="B1:CG13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="55" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="BL1" colorId="64" zoomScale="90" zoomScaleNormal="55" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BP5" activeCellId="0" sqref="BP5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="46" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="85" min="4" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="46" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="85" min="4" style="0" width="20.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="86" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
delimiter  is ',' and not ', '
</commit_message>
<xml_diff>
--- a/Projects/CCKH/Data/Template_New.xlsx
+++ b/Projects/CCKH/Data/Template_New.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,7 @@
     <sheet name="COOLER" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">AVAILABILITY!$B$5:$CH$19</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">AVAILABILITY!$B$5:$CH$18</definedName>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">COOLER!$B$5:$S$5</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$T$32</definedName>
     <definedName function="false" hidden="false" name="Apples" vbProcedure="false">#REF!</definedName>
@@ -37,17 +37,19 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$T$32</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$T$32</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$T$32</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">AVAILABILITY!$B$5:$CH$18</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$19</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$18</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$19</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$18</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$19</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$18</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$19</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$T$32</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">AVAILABILITY!$B$5:$CH$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$19</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$18</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">AVAILABILITY!$B$5:$CH$18</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">VISIBILITY!$B$5:$F$5</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">COOLER!$B$5:$S$5</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">COOLER!$B$5:$S$5</definedName>
@@ -60,6 +62,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">COOLER!$B$5:$S$5</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">COOLER!$B$5:$S$5</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">COOLER!$B$5:$S$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">COOLER!$B$5:$S$5</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -481,7 +484,7 @@
     <t xml:space="preserve">Min. Cooler SOVI</t>
   </si>
   <si>
-    <t xml:space="preserve">KO Cooler, Cold</t>
+    <t xml:space="preserve">KO Cooler,Cold</t>
   </si>
   <si>
     <t xml:space="preserve">Empty,Irrelevant</t>
@@ -502,7 +505,7 @@
     <t xml:space="preserve">Warm</t>
   </si>
   <si>
-    <t xml:space="preserve">KH-Tradi. Grocery_Gold, KH-Mini Wholesaler_Gold, KH-At Work/Offices_Gold, KH-BBQ/Soup/Beer Gdn_Gold, KH-Café Shop_Gold, KH-Canteen-Edu/Fact._Gold, KH-Cash &amp; Carry_Gold, KH-Cinema_Gold, KH-CVS_Gold, KH-Drinking Stalls_Gold, KH-Entertainment_Gold, KH-Fitness Center_Gold, KH-Food Court_Gold, KH-Food Stalls_Gold, KH-GH./Mini-Hotel_Gold, KH-Hotel(4Stars Up)_Gold, KH-Hypermarket_Gold, KH-Internet/E-Game_Gold, KH-KA Pharmacy _Gold, KH-KTV/Night Club_Gold, KH-Massage/Spa_Gold, KH-Mobile Premix_Gold, KH-Petrol Mart_Gold, KH-QSR_Gold, KH-Restaurants_Gold, KH-Sport Club_Gold, KH-Supermarket_Gold, KH-Tradi. Pharmacy_Gold, KH-Tradi. Grocery_Silver, KH-At Work/Offices_Silver, KH-BBQ/Soup/Beer Gdn_Silver, KH-Café Shop_Silver, KH-Canteen-Edu/Fact._Silver, KH-Cash &amp; Carry_Silver, KH-Cinema_Silver, KH-CVS_Silver, KH-Drinking Stalls_Silver, KH-Entertainment_Silver, KH-Fitness Center_Silver, KH-Food Court_Silver, KH-Food Stalls_Silver, KH-GH./Mini-Hotel_Silver, KH-Hotel(4Stars Up)_Silver, KH-Hypermarket_Silver, KH-Internet/E-Game_Silver, KH-KA Pharmacy _Silver, KH-KTV/Night Club_Silver, KH-Massage/Spa_Silver, KH-Mobile Premix_Silver, KH-Petrol Mart_Silver, KH-QSR_Silver, KH-Restaurants_Silver, KH-Sport Club_Silver, KH-Supermarket_Silver, KH-Tradi. Pharmacy_Silver, KH-Tradi. Grocery_Bronze, KH-At Work/Offices_Bronze, KH-BBQ/Soup/Beer Gdn_Bronze, KH-Café Shop_Bronze, KH-Canteen-Edu/Fact._Bronze, KH-Cash &amp; Carry_Bronze, KH-Cinema_Bronze, KH-CVS_Bronze, KH-Drinking Stalls_Bronze, KH-Entertainment_Bronze, KH-Fitness Center_Bronze, KH-Food Court_Bronze, KH-Food Stalls_Bronze, KH-GH./Mini-Hotel_Bronze, KH-Hotel(4Stars Up)_Bronze, KH-Hypermarket_Bronze, KH-Internet/E-Game_Bronze, KH-KA Pharmacy _Bronze, KH-KTV/Night Club_Bronze, KH-Massage/Spa_Bronze, KH-Mobile Premix_Bronze, KH-Petrol Mart_Bronze, KH-QSR_Bronze, KH-Restaurants_Bronze, KH-Sport Club_Bronze, KH-Supermarket_Bronze, KH-Tradi. Pharmacy_Bronze</t>
+    <t xml:space="preserve">KH-Tradi. Grocery_Gold,KH-Mini Wholesaler_Gold,KH-At Work/Offices_Gold,KH-BBQ/Soup/Beer Gdn_Gold,KH-Café Shop_Gold,KH-Canteen-Edu/Fact._Gold,KH-Cash &amp; Carry_Gold,KH-Cinema_Gold,KH-CVS_Gold,KH-Drinking Stalls_Gold,KH-Entertainment_Gold,KH-Fitness Center_Gold,KH-Food Court_Gold,KH-Food Stalls_Gold,KH-GH./Mini-Hotel_Gold,KH-Hotel(4Stars Up)_Gold,KH-Hypermarket_Gold,KH-Internet/E-Game_Gold,KH-KA Pharmacy _Gold,KH-KTV/Night Club_Gold,KH-Massage/Spa_Gold,KH-Mobile Premix_Gold,KH-Petrol Mart_Gold,KH-QSR_Gold,KH-Restaurants_Gold,KH-Sport Club_Gold,KH-Supermarket_Gold,KH-Tradi. Pharmacy_Gold,KH-Tradi. Grocery_Silver,KH-At Work/Offices_Silver,KH-BBQ/Soup/Beer Gdn_Silver,KH-Café Shop_Silver,KH-Canteen-Edu/Fact._Silver,KH-Cash &amp; Carry_Silver,KH-Cinema_Silver,KH-CVS_Silver,KH-Drinking Stalls_Silver,KH-Entertainment_Silver,KH-Fitness Center_Silver,KH-Food Court_Silver,KH-Food Stalls_Silver,KH-GH./Mini-Hotel_Silver,KH-Hotel(4Stars Up)_Silver,KH-Hypermarket_Silver,KH-Internet/E-Game_Silver,KH-KA Pharmacy _Silver,KH-KTV/Night Club_Silver,KH-Massage/Spa_Silver,KH-Mobile Premix_Silver,KH-Petrol Mart_Silver,KH-QSR_Silver,KH-Restaurants_Silver,KH-Sport Club_Silver,KH-Supermarket_Silver,KH-Tradi. Pharmacy_Silver,KH-Tradi. Grocery_Bronze,KH-At Work/Offices_Bronze,KH-BBQ/Soup/Beer Gdn_Bronze,KH-Café Shop_Bronze,KH-Canteen-Edu/Fact._Bronze,KH-Cash &amp; Carry_Bronze,KH-Cinema_Bronze,KH-CVS_Bronze,KH-Drinking Stalls_Bronze,KH-Entertainment_Bronze,KH-Fitness Center_Bronze,KH-Food Court_Bronze,KH-Food Stalls_Bronze,KH-GH./Mini-Hotel_Bronze,KH-Hotel(4Stars Up)_Bronze,KH-Hypermarket_Bronze,KH-Internet/E-Game_Bronze,KH-KA Pharmacy _Bronze,KH-KTV/Night Club_Bronze,KH-Massage/Spa_Bronze,KH-Mobile Premix_Bronze,KH-Petrol Mart_Bronze,KH-QSR_Bronze,KH-Restaurants_Bronze,KH-Sport Club_Bronze,KH-Supermarket_Bronze,KH-Tradi. Pharmacy_Bronze</t>
   </si>
   <si>
     <t xml:space="preserve">Cooler Club</t>
@@ -987,8 +990,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="0%"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
     <numFmt numFmtId="168" formatCode="@"/>
@@ -1278,7 +1281,7 @@
     </border>
   </borders>
   <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1296,96 +1299,96 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="49">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1393,23 +1396,23 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1425,11 +1428,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="13" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1437,39 +1440,39 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1481,11 +1484,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1518,83 +1521,167 @@
   <dxfs count="8">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <color rgb="FF000000"/>
+        <u val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="00FFFFFF"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <color rgb="FF000000"/>
+        <u val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="00FFFFFF"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <name val="Calibri"/>
+        <charset val="177"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <color rgb="FF000000"/>
+        <u val="none"/>
       </font>
+      <numFmt numFmtId="165" formatCode="General"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="00FFFFFF"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <border diagonalUp="false" diagonalDown="false">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <diagonal/>
+      </border>
+      <protection locked="true" hidden="false"/>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <color rgb="FF000000"/>
+        <u val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="00FFFFFF"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <color rgb="FF000000"/>
+        <u val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="00FFFFFF"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <color rgb="FF000000"/>
+        <u val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="00FFFFFF"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <color rgb="FF000000"/>
+        <u val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="00FFFFFF"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -1679,29 +1766,29 @@
   </sheetPr>
   <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="86" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="86" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A28" activeCellId="3" sqref="A26 A30:A31 H24 A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.17004048583"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.3117408906883"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.4574898785425"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="80.9838056680162"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="55.5951417004049"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6356275303644"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6720647773279"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="81.7327935222672"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="56.0242914979757"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="43.7044534412956"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="44.0242914979757"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="38.5627530364372"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="79.0526315789474"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="79.6963562753036"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="30.8502024291498"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="9.10526315789474"/>
@@ -3198,21 +3285,19 @@
   </sheetPr>
   <dimension ref="B1:CH19"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="70" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="70" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane xSplit="0" ySplit="4" topLeftCell="E5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E28" activeCellId="0" sqref="E28"/>
+      <selection pane="bottomLeft" activeCell="E28" activeCellId="3" sqref="A26 A30:A31 H24 E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="31.3846153846154"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.8825910931174"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2307692307692"/>
-    <col collapsed="false" hidden="false" max="86" min="5" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.2024291497976"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="86" min="5" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="87" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -7268,7 +7353,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B5:CH19"/>
+  <autoFilter ref="B5:CH18"/>
   <mergeCells count="8">
     <mergeCell ref="B3:D4"/>
     <mergeCell ref="E3:CH3"/>
@@ -7352,13 +7437,13 @@
   <dimension ref="B1:CF8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="AS1" colorId="64" zoomScale="90" zoomScaleNormal="85" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AY5" activeCellId="0" sqref="AY5"/>
+      <selection pane="topLeft" activeCell="AY5" activeCellId="3" sqref="A26 A30:A31 H24 AY5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="60.3076923076923"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="60.8421052631579"/>
     <col collapsed="false" hidden="false" max="84" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="85" style="0" width="8.57085020242915"/>
   </cols>
@@ -8586,15 +8671,15 @@
   <dimension ref="B1:CG13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="BL1" colorId="64" zoomScale="90" zoomScaleNormal="55" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BP5" activeCellId="0" sqref="BP5"/>
+      <selection pane="topLeft" activeCell="BP5" activeCellId="3" sqref="A26 A30:A31 H24 BP5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="44" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="85" min="4" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="44" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="85" min="4" style="0" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="86" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>